<commit_message>
qPCR templates and reports; COI databases
</commit_message>
<xml_diff>
--- a/docs/eDNA qPCR/example input/client_metadata_example.xlsx
+++ b/docs/eDNA qPCR/example input/client_metadata_example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BoxDrive\Box\Science\Fisheries\Projects\eDNA\Contract Work Resources\qPCR\example input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BoxDrive\Box\Science\Fisheries\github\resources\docs\eDNA qPCR\example input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B3A9C4-DE2E-4C73-BBE5-322B95FE51D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99AE8F0-9284-4441-B810-6C43434E3F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,7 +90,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="291">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="290">
   <si>
     <t>EPS_DMF</t>
   </si>
@@ -939,9 +939,6 @@
   </si>
   <si>
     <t>KCK_NRS</t>
-  </si>
-  <si>
-    <t>SKR_PFB_2</t>
   </si>
   <si>
     <t>WRN_PVD</t>
@@ -1360,8 +1357,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E207"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2518,7 +2515,7 @@
         <v>45343</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>283</v>
+        <v>53</v>
       </c>
       <c r="C77" s="6" t="s">
         <v>149</v>
@@ -2533,7 +2530,7 @@
         <v>45343</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C78" s="6" t="s">
         <v>150</v>
@@ -2548,7 +2545,7 @@
         <v>45343</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C79" s="6" t="s">
         <v>151</v>
@@ -2563,7 +2560,7 @@
         <v>45343</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C80" s="6" t="s">
         <v>152</v>
@@ -2578,7 +2575,7 @@
         <v>45343</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C81" s="6" t="s">
         <v>153</v>
@@ -3748,7 +3745,7 @@
         <v>45373</v>
       </c>
       <c r="B159" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C159" s="6" t="s">
         <v>231</v>
@@ -3763,7 +3760,7 @@
         <v>45373</v>
       </c>
       <c r="B160" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C160" s="6" t="s">
         <v>232</v>
@@ -3778,7 +3775,7 @@
         <v>45373</v>
       </c>
       <c r="B161" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C161" s="6" t="s">
         <v>233</v>
@@ -3793,7 +3790,7 @@
         <v>45373</v>
       </c>
       <c r="B162" s="4" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C162" s="6" t="s">
         <v>234</v>
@@ -3898,7 +3895,7 @@
         <v>45440</v>
       </c>
       <c r="B169" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="C169" s="6" t="s">
         <v>241</v>
@@ -3973,7 +3970,7 @@
         <v>45440</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C174" s="6" t="s">
         <v>246</v>
@@ -3988,7 +3985,7 @@
         <v>45440</v>
       </c>
       <c r="B175" s="4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C175" s="6" t="s">
         <v>247</v>
@@ -4243,7 +4240,7 @@
         <v>45440</v>
       </c>
       <c r="B192" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C192" s="6" t="s">
         <v>264</v>
@@ -4258,7 +4255,7 @@
         <v>45440</v>
       </c>
       <c r="B193" s="4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C193" s="6" t="s">
         <v>265</v>
@@ -4333,7 +4330,7 @@
         <v>45440</v>
       </c>
       <c r="B198" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C198" s="6" t="s">
         <v>270</v>
@@ -4348,7 +4345,7 @@
         <v>45440</v>
       </c>
       <c r="B199" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C199" s="6" t="s">
         <v>271</v>
@@ -4363,7 +4360,7 @@
         <v>45440</v>
       </c>
       <c r="B200" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C200" s="6" t="s">
         <v>272</v>
@@ -4378,7 +4375,7 @@
         <v>45440</v>
       </c>
       <c r="B201" s="4" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C201" s="6" t="s">
         <v>273</v>
@@ -4393,7 +4390,7 @@
         <v>45440</v>
       </c>
       <c r="B202" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C202" s="6" t="s">
         <v>274</v>
@@ -4408,7 +4405,7 @@
         <v>45440</v>
       </c>
       <c r="B203" s="4" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C203" s="6" t="s">
         <v>275</v>

</xml_diff>